<commit_message>
Introducing the notebook to the  project.
</commit_message>
<xml_diff>
--- a/data/Sorbic_Benzoic.xlsx
+++ b/data/Sorbic_Benzoic.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="93" documentId="8_{8FD17947-3392-402B-B6AC-BAC5457FF132}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{521E32B3-B831-413D-ACD5-FE278229E4FC}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="900" windowWidth="18705" windowHeight="10020" activeTab="2" xr2:uid="{26731E02-B61E-284A-8F48-A390778ACEA0}"/>
+    <workbookView xWindow="1110" yWindow="375" windowWidth="18705" windowHeight="10020" activeTab="2" xr2:uid="{26731E02-B61E-284A-8F48-A390778ACEA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sorbic2" sheetId="4" r:id="rId1"/>
@@ -1570,7 +1570,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>